<commit_message>
Add 2 previous papers
</commit_message>
<xml_diff>
--- a/excel/paper_list.xlsx
+++ b/excel/paper_list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b91426b3d7947356/RESEARCH/Rinko_Document_2023A (Lian)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b91426b3d7947356/RESEARCH/Workspace/Awesome-Articulated-Object-Understanding/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="627" documentId="11_AD4DA82427541F7ACA7EB8D328C939426BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68FD2773-5FE3-4D41-9091-D7A55CDECA19}"/>
+  <xr:revisionPtr revIDLastSave="759" documentId="11_AD4DA82427541F7ACA7EB8D328C939426BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8B5A39C-30CC-428F-A154-C4DB3192355D}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-108" windowWidth="13176" windowHeight="22656" tabRatio="531" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="1920" windowWidth="2031" windowHeight="3420" tabRatio="531" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dataset" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="363">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,10 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dataset, Articulation, Reconstruct</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A-SDF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,9 +158,6 @@
     <t>Ditto: Building Digital Twins of Articulated Objects from Interaction</t>
   </si>
   <si>
-    <t>Ditto</t>
-  </si>
-  <si>
     <t>Shape2Motion</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Ditto in the house</t>
-  </si>
-  <si>
     <t>ICRA 2023</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -192,9 +183,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CARTO</t>
-  </si>
-  <si>
     <t>FlowBot3D: Learning 3D Articulation Flow to Manipulate Articulated Objects</t>
   </si>
   <si>
@@ -246,9 +234,6 @@
     <t>CAPTRA</t>
   </si>
   <si>
-    <t>Nothing But Geometric Constraints: A Model-Free Method for Articulated Object Pose Estimation</t>
-  </si>
-  <si>
     <t>GC-Pose</t>
   </si>
   <si>
@@ -292,9 +277,6 @@
   </si>
   <si>
     <t>RBO</t>
-  </si>
-  <si>
-    <t>Tzionas etc.</t>
   </si>
   <si>
     <t>Sturm etc.</t>
@@ -1405,6 +1387,129 @@
       </rPr>
       <t xml:space="preserve"> Refinement</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PartNet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPDReal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPDSynth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOCS-REAL275</t>
+  </si>
+  <si>
+    <t>YCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RBO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Objaverse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Objaverse-XL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nothing But Geometric Constraints: A Model-Free Method for Articulated Object Pose Estimation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dataset, Articulation, Reconstruction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unsupervised Kinematic Motion Detection for Part-segmented 3D Shape Collections</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrobeNet: Category-Level Multiview Reconstruction of Articulated Objects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrobeNet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CARTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ditto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tzionas etc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ditto in the house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIGGRAPH 2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2206.08497</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UKMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/xxh43/ukmd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D models of manufactured objects are important for populating virtual worlds and for synthetic data generation for vision and robotics. To be most useful, such objects should be articulated: their parts should move when interacted with. While articulated object datasets exist, creating them is labor-intensive. Learning-based prediction of part motions can help, but all existing methods require annotated training data. In this paper, we present an unsupervised approach for discovering articulated motions in a part-segmented 3D shape collection. Our approach is based on a concept we call category closure: any valid articulation of an object's parts should keep the object in the same semantic category (e.g. a chair stays a chair). We operationalize this concept with an algorithm that optimizes a shape's part motion parameters such that it can transform into other shapes in the collection. We evaluate our approach by using it to re-discover part motions from the PartNet-Mobility dataset. For almost all shape categories, our method's predicted motion parameters have low error with respect to ground truth annotations, outperforming two supervised motion prediction methods.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single shape + segmentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Candidate + 2 stage optimization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2105.08016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arxiv 2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://dzhange.github.io/StrobeNet/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A set of sparse images</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SegNet, IF-Net</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAOCS + Reconstruction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We present StrobeNet, a method for category-level 3D reconstruction of articulating objects from one or more unposed RGB images. Reconstructing general articulating object categories % has important applications, but is challenging since objects can have wide variation in shape, articulation, appearance and topology. We address this by building on the idea of category-level articulation canonicalization -- mapping observations to a canonical articulation which enables correspondence-free multiview aggregation. Our end-to-end trainable neural network estimates feature-enriched canonical 3D point clouds, articulation joints, and part segmentation from one or more unposed images of an object. These intermediate estimates are used to generate a final implicit 3D reconstruction.Our approach reconstructs objects even when they are observed in different articulations in images with large baselines, and animation of reconstructed shapes. Quantitative and qualitative evaluations on different object categories show that our method is able to achieve high reconstruction accuracy, especially as more views are added.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1475,12 +1580,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1496,7 +1607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1513,7 +1624,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1801,11 +1921,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1817,9 +1937,9 @@
     <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.2109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="23.2109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="31.640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="47.2109375" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1837,13 +1957,13 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -1852,10 +1972,10 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>13</v>
@@ -1864,240 +1984,240 @@
         <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="6">
         <v>2023</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="6">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>123</v>
+      <c r="M2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>348</v>
       </c>
       <c r="C3" s="2">
         <v>2023</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C4" s="2">
         <v>2023</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="8" customFormat="1" ht="18.45" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2023</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18.45" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2023</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C6" s="2">
         <v>2023</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2">
         <v>2023</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2105,22 +2225,22 @@
         <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -2137,13 +2257,13 @@
         <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>13</v>
@@ -2155,81 +2275,81 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2022</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2">
         <v>2022</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
@@ -2238,157 +2358,157 @@
         <v>6</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2">
         <v>2022</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>5</v>
+        <v>330</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2022</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>204</v>
+      <c r="M12" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
         <v>2022</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2">
         <v>2022</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2396,7 +2516,7 @@
         <v>5</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>11</v>
@@ -2408,113 +2528,113 @@
         <v>6</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C15" s="2">
         <v>2022</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C16" s="2">
         <v>2022</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2">
         <v>2022</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -2522,125 +2642,125 @@
         <v>5</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="M17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="6">
         <v>2022</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="E18" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K18" s="2">
+      <c r="I18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="6">
         <v>1</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>230</v>
+      <c r="L18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2">
         <v>2021</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K19" s="2">
         <v>1</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C20" s="2">
         <v>2021</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2649,34 +2769,34 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2">
         <v>2021</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -2684,54 +2804,54 @@
         <v>5</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2">
         <v>2021</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="K22" s="2">
         <v>1</v>
@@ -2740,115 +2860,115 @@
         <v>6</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2">
         <v>2021</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K23" s="2">
         <v>1</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="N23" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="6">
+        <v>1</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="N24" s="6" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="2">
-        <v>2021</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2">
         <v>2021</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2856,10 +2976,10 @@
         <v>5</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K25" s="2">
         <v>2</v>
@@ -2868,10 +2988,10 @@
         <v>6</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -2888,16 +3008,16 @@
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2907,24 +3027,24 @@
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>340</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2">
         <v>2020</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2932,83 +3052,83 @@
         <v>5</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K27" s="2">
         <v>2</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C28" s="2">
         <v>2020</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K28" s="2">
         <v>2</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2">
         <v>2020</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -3016,115 +3136,115 @@
         <v>5</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2">
         <v>2019</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="K30" s="2">
         <v>1</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2">
         <v>2019</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K31" s="2">
         <v>1</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2">
         <v>2019</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -3132,127 +3252,127 @@
         <v>5</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K32" s="2">
         <v>1</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2">
         <v>2019</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C34" s="2">
         <v>2018</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2">
         <v>2018</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>5</v>
@@ -3263,24 +3383,24 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2">
         <v>2017</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -3288,87 +3408,87 @@
         <v>5</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C37" s="1">
         <v>2017</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C38" s="6">
         <v>2016</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2" t="s">
+      <c r="D38" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>324</v>
+      <c r="I38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -3382,14 +3502,14 @@
         <v>2015</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="3" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>13</v>
@@ -3402,24 +3522,24 @@
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C40" s="2">
         <v>2009</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -3429,14 +3549,90 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3528,8 +3724,143 @@
     <hyperlink ref="E39" r:id="rId81" xr:uid="{4BD5D06C-8412-4618-B275-23234C0E3157}"/>
     <hyperlink ref="G39" r:id="rId82" xr:uid="{4B6FC557-C65C-48DE-9457-46A51DF77291}"/>
     <hyperlink ref="E40" r:id="rId83" xr:uid="{1E0CFEA1-115B-4549-AEC6-3A5F4CC9BF62}"/>
+    <hyperlink ref="E41" r:id="rId84" xr:uid="{5BE0236A-6B78-408B-A1E9-9CEE8E361C8B}"/>
+    <hyperlink ref="F41" r:id="rId85" xr:uid="{9B713C4D-8D39-4B99-ADA9-4A7174EA969E}"/>
+    <hyperlink ref="E42" r:id="rId86" xr:uid="{7741AAD2-3EE4-481A-9F89-1B2EEA713AA1}"/>
+    <hyperlink ref="G42" r:id="rId87" xr:uid="{A947AEA1-F91D-4B4C-BD05-200FCB9E26DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId84"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId88"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2C6482-5B84-48E2-82DE-D21D277A9130}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="8.78515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B37">
+    <sortCondition descending="1" ref="B1:B37"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>